<commit_message>
Feebased With new data for 254
</commit_message>
<xml_diff>
--- a/NSDC_Web_Automation/UploadFiles/CandidateEnrollmentList.xlsx
+++ b/NSDC_Web_Automation/UploadFiles/CandidateEnrollmentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trans\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CA83358-BA71-4D2D-9880-2876E64E2C20}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F016A2F8-4AAC-44EF-A11E-E84AD2E7C6D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="269">
   <si>
     <t>Common Candidate Details</t>
   </si>
@@ -449,336 +449,360 @@
     <t>Mr</t>
   </si>
   <si>
+    <t>mahesh</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>01/04/2000</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Single/Unmarried</t>
+  </si>
+  <si>
+    <t>Ganesh</t>
+  </si>
+  <si>
+    <t>Sunaina</t>
+  </si>
+  <si>
+    <t>Golu</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>37 Mall Road</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>110046</t>
+  </si>
+  <si>
+    <t>Shahdara</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>8712345345</t>
+  </si>
+  <si>
+    <t>01123459890</t>
+  </si>
+  <si>
+    <t>123456@gmail.com</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>bulkupload</t>
+  </si>
+  <si>
+    <t>Created by Training Partner, TP_001564</t>
+  </si>
+  <si>
+    <t>CAN_021112</t>
+  </si>
+  <si>
+    <t>priya</t>
+  </si>
+  <si>
+    <t>01/04/1988</t>
+  </si>
+  <si>
+    <t>25 Mall Road</t>
+  </si>
+  <si>
+    <t>110034</t>
+  </si>
+  <si>
+    <t>01123459878</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>CAN_021125</t>
+  </si>
+  <si>
+    <t>shashank</t>
+  </si>
+  <si>
+    <t>01/04/1990</t>
+  </si>
+  <si>
+    <t>27 Mall Road</t>
+  </si>
+  <si>
+    <t>110036</t>
+  </si>
+  <si>
+    <t>01123459880</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>CAN_021115</t>
+  </si>
+  <si>
+    <t>sheetal</t>
+  </si>
+  <si>
+    <t>01/04/1989</t>
+  </si>
+  <si>
+    <t>26 Mall Road</t>
+  </si>
+  <si>
+    <t>110035</t>
+  </si>
+  <si>
+    <t>01123459879</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>CAN_021114</t>
+  </si>
+  <si>
+    <t>pampa</t>
+  </si>
+  <si>
+    <t>01/04/1992</t>
+  </si>
+  <si>
+    <t>29 Mall Road</t>
+  </si>
+  <si>
+    <t>110038</t>
+  </si>
+  <si>
+    <t>01123459882</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>CAN_021117</t>
+  </si>
+  <si>
+    <t>kirti</t>
+  </si>
+  <si>
+    <t>01/04/1986</t>
+  </si>
+  <si>
+    <t>23 Mall Road</t>
+  </si>
+  <si>
+    <t>110032</t>
+  </si>
+  <si>
+    <t>01123459876</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>CAN_021113</t>
+  </si>
+  <si>
+    <t>roshni</t>
+  </si>
+  <si>
+    <t>01/04/1991</t>
+  </si>
+  <si>
+    <t>28 Mall Road</t>
+  </si>
+  <si>
+    <t>110037</t>
+  </si>
+  <si>
+    <t>01123459881</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>CAN_021116</t>
+  </si>
+  <si>
+    <t>sameena</t>
+  </si>
+  <si>
+    <t>01/04/1993</t>
+  </si>
+  <si>
+    <t>30 Mall Road</t>
+  </si>
+  <si>
+    <t>110039</t>
+  </si>
+  <si>
+    <t>01123459883</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>CAN_021118</t>
+  </si>
+  <si>
+    <t>leela</t>
+  </si>
+  <si>
+    <t>01/04/1996</t>
+  </si>
+  <si>
+    <t>33 Mall Road</t>
+  </si>
+  <si>
+    <t>110042</t>
+  </si>
+  <si>
+    <t>01123459886</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>CAN_021121</t>
+  </si>
+  <si>
+    <t>preksha</t>
+  </si>
+  <si>
+    <t>01/04/1997</t>
+  </si>
+  <si>
+    <t>34 Mall Road</t>
+  </si>
+  <si>
+    <t>110043</t>
+  </si>
+  <si>
+    <t>01123459887</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>CAN_021122</t>
+  </si>
+  <si>
+    <t>prema</t>
+  </si>
+  <si>
+    <t>01/04/1995</t>
+  </si>
+  <si>
+    <t>32 Mall Road</t>
+  </si>
+  <si>
+    <t>110041</t>
+  </si>
+  <si>
+    <t>01123459885</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>CAN_021120</t>
+  </si>
+  <si>
     <t>Harshit</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>01/04/1997</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>Single/Unmarried</t>
-  </si>
-  <si>
-    <t>Ganesh</t>
-  </si>
-  <si>
-    <t>Sunaina</t>
-  </si>
-  <si>
-    <t>Golu</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Hindu</t>
+    <t>01/04/1999</t>
   </si>
   <si>
     <t>36 Mall Road</t>
   </si>
   <si>
-    <t>New Delhi</t>
-  </si>
-  <si>
     <t>110045</t>
   </si>
   <si>
-    <t>Shahdara</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>8712345345</t>
-  </si>
-  <si>
     <t>01123459889</t>
   </si>
   <si>
-    <t>123456@gmail.com</t>
-  </si>
-  <si>
     <t>34</t>
   </si>
   <si>
     <t>114</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Graduate</t>
-  </si>
-  <si>
-    <t>bulkupload</t>
-  </si>
-  <si>
-    <t>Created by Training Partner, TP_002652</t>
-  </si>
-  <si>
-    <t>CAN_025936</t>
-  </si>
-  <si>
-    <t>mahesh</t>
+    <t>CAN_021124</t>
+  </si>
+  <si>
+    <t>pooja</t>
+  </si>
+  <si>
+    <t>01/04/1994</t>
+  </si>
+  <si>
+    <t>31 Mall Road</t>
+  </si>
+  <si>
+    <t>110040</t>
+  </si>
+  <si>
+    <t>01123459884</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>CAN_021119</t>
+  </si>
+  <si>
+    <t>kishore</t>
   </si>
   <si>
     <t>01/04/1998</t>
   </si>
   <si>
-    <t>37 Mall Road</t>
-  </si>
-  <si>
-    <t>110046</t>
-  </si>
-  <si>
-    <t>01123459890</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>CAN_025923</t>
-  </si>
-  <si>
-    <t>pallavi</t>
-  </si>
-  <si>
-    <t>01/04/1985</t>
-  </si>
-  <si>
-    <t>24 Mall Road</t>
-  </si>
-  <si>
-    <t>110033</t>
-  </si>
-  <si>
-    <t>01123459877</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>CAN_025925</t>
-  </si>
-  <si>
-    <t>priya</t>
-  </si>
-  <si>
-    <t>01/04/1986</t>
-  </si>
-  <si>
-    <t>25 Mall Road</t>
-  </si>
-  <si>
-    <t>110034</t>
-  </si>
-  <si>
-    <t>01123459878</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>CAN_025926</t>
-  </si>
-  <si>
-    <t>kirti</t>
-  </si>
-  <si>
-    <t>01/04/1984</t>
-  </si>
-  <si>
-    <t>23 Mall Road</t>
-  </si>
-  <si>
-    <t>110032</t>
-  </si>
-  <si>
-    <t>01123459876</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>CAN_025924</t>
-  </si>
-  <si>
-    <t>shashank</t>
-  </si>
-  <si>
-    <t>01/04/1988</t>
-  </si>
-  <si>
-    <t>27 Mall Road</t>
-  </si>
-  <si>
-    <t>110036</t>
-  </si>
-  <si>
-    <t>01123459880</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>CAN_025927</t>
-  </si>
-  <si>
-    <t>pooja</t>
-  </si>
-  <si>
-    <t>01/04/1992</t>
-  </si>
-  <si>
-    <t>31 Mall Road</t>
-  </si>
-  <si>
-    <t>110040</t>
-  </si>
-  <si>
-    <t>01123459884</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>CAN_025931</t>
-  </si>
-  <si>
-    <t>leela</t>
-  </si>
-  <si>
-    <t>01/04/1994</t>
-  </si>
-  <si>
-    <t>33 Mall Road</t>
-  </si>
-  <si>
-    <t>110042</t>
-  </si>
-  <si>
-    <t>01123459886</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>CAN_025933</t>
-  </si>
-  <si>
-    <t>pampa</t>
-  </si>
-  <si>
-    <t>01/04/1990</t>
-  </si>
-  <si>
-    <t>29 Mall Road</t>
-  </si>
-  <si>
-    <t>110038</t>
-  </si>
-  <si>
-    <t>01123459882</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>CAN_025929</t>
-  </si>
-  <si>
-    <t>sameena</t>
-  </si>
-  <si>
-    <t>01/04/1991</t>
-  </si>
-  <si>
-    <t>30 Mall Road</t>
-  </si>
-  <si>
-    <t>110039</t>
-  </si>
-  <si>
-    <t>01123459883</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
-    <t>CAN_025930</t>
-  </si>
-  <si>
-    <t>roshni</t>
-  </si>
-  <si>
-    <t>01/04/1989</t>
-  </si>
-  <si>
-    <t>28 Mall Road</t>
-  </si>
-  <si>
-    <t>110037</t>
-  </si>
-  <si>
-    <t>01123459881</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>CAN_025928</t>
-  </si>
-  <si>
-    <t>preksha</t>
-  </si>
-  <si>
-    <t>01/04/1995</t>
-  </si>
-  <si>
-    <t>34 Mall Road</t>
-  </si>
-  <si>
-    <t>110043</t>
-  </si>
-  <si>
-    <t>01123459887</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>CAN_025934</t>
-  </si>
-  <si>
-    <t>kishore</t>
-  </si>
-  <si>
-    <t>01/04/1996</t>
-  </si>
-  <si>
     <t>35 Mall Road</t>
   </si>
   <si>
@@ -794,37 +818,16 @@
     <t>113</t>
   </si>
   <si>
-    <t>CAN_025935</t>
-  </si>
-  <si>
-    <t>prema</t>
-  </si>
-  <si>
-    <t>01/04/1993</t>
-  </si>
-  <si>
-    <t>32 Mall Road</t>
-  </si>
-  <si>
-    <t>110041</t>
-  </si>
-  <si>
-    <t>01123459885</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>CAN_025932</t>
-  </si>
-  <si>
-    <t>sheetal</t>
-  </si>
-  <si>
-    <t>CAN_025937</t>
+    <t>CAN_021123</t>
+  </si>
+  <si>
+    <t>meena</t>
+  </si>
+  <si>
+    <t>01/04/1983</t>
+  </si>
+  <si>
+    <t>CAN_021126</t>
   </si>
   <si>
     <t>Completed</t>
@@ -1425,7 +1428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMG19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AL4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AY5" sqref="AY5:AY19"/>
     </sheetView>
   </sheetViews>
@@ -2423,7 +2426,7 @@
         <v>165</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY5" s="1">
         <v>100</v>
@@ -2521,10 +2524,10 @@
         <v>159</v>
       </c>
       <c r="AD6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE6" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="AE6" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>162</v>
@@ -2539,13 +2542,13 @@
         <v>165</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY6" s="1">
         <v>100</v>
       </c>
       <c r="CE6" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:89" x14ac:dyDescent="0.25">
@@ -2553,13 +2556,13 @@
         <v>140</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>144</v>
@@ -2586,7 +2589,7 @@
         <v>151</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>153</v>
@@ -2598,7 +2601,7 @@
         <v>144</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>155</v>
@@ -2607,7 +2610,7 @@
         <v>156</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>153</v>
@@ -2616,7 +2619,7 @@
         <v>144</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>144</v>
@@ -2631,16 +2634,16 @@
         <v>157</v>
       </c>
       <c r="AB7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AC7" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AF7" s="1" t="s">
         <v>162</v>
@@ -2655,13 +2658,13 @@
         <v>165</v>
       </c>
       <c r="AX7" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY7" s="1">
         <v>100</v>
       </c>
       <c r="CE7" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:89" x14ac:dyDescent="0.25">
@@ -2669,13 +2672,13 @@
         <v>140</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>144</v>
@@ -2702,7 +2705,7 @@
         <v>151</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>153</v>
@@ -2714,7 +2717,7 @@
         <v>144</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>155</v>
@@ -2723,7 +2726,7 @@
         <v>156</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>153</v>
@@ -2732,7 +2735,7 @@
         <v>144</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="X8" s="1" t="s">
         <v>144</v>
@@ -2747,16 +2750,16 @@
         <v>157</v>
       </c>
       <c r="AB8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC8" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>162</v>
@@ -2771,13 +2774,13 @@
         <v>165</v>
       </c>
       <c r="AX8" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY8" s="1">
         <v>100</v>
       </c>
       <c r="CE8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:89" x14ac:dyDescent="0.25">
@@ -2785,13 +2788,13 @@
         <v>140</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>144</v>
@@ -2818,7 +2821,7 @@
         <v>151</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>153</v>
@@ -2830,7 +2833,7 @@
         <v>144</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>155</v>
@@ -2839,7 +2842,7 @@
         <v>156</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>153</v>
@@ -2848,7 +2851,7 @@
         <v>144</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="X9" s="1" t="s">
         <v>144</v>
@@ -2863,16 +2866,16 @@
         <v>157</v>
       </c>
       <c r="AB9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC9" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF9" s="1" t="s">
         <v>162</v>
@@ -2887,13 +2890,13 @@
         <v>165</v>
       </c>
       <c r="AX9" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY9" s="1">
         <v>100</v>
       </c>
       <c r="CE9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:89" x14ac:dyDescent="0.25">
@@ -2901,13 +2904,13 @@
         <v>140</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>144</v>
@@ -2934,7 +2937,7 @@
         <v>151</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>153</v>
@@ -2946,7 +2949,7 @@
         <v>144</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>155</v>
@@ -2955,7 +2958,7 @@
         <v>156</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>153</v>
@@ -2964,7 +2967,7 @@
         <v>144</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="X10" s="1" t="s">
         <v>144</v>
@@ -2979,16 +2982,16 @@
         <v>157</v>
       </c>
       <c r="AB10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AC10" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF10" s="1" t="s">
         <v>162</v>
@@ -3003,13 +3006,13 @@
         <v>165</v>
       </c>
       <c r="AX10" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY10" s="1">
         <v>100</v>
       </c>
       <c r="CE10" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:89" x14ac:dyDescent="0.25">
@@ -3017,13 +3020,13 @@
         <v>140</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>144</v>
@@ -3050,7 +3053,7 @@
         <v>151</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>153</v>
@@ -3062,7 +3065,7 @@
         <v>144</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>155</v>
@@ -3071,7 +3074,7 @@
         <v>156</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>153</v>
@@ -3080,7 +3083,7 @@
         <v>144</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="X11" s="1" t="s">
         <v>144</v>
@@ -3095,16 +3098,16 @@
         <v>157</v>
       </c>
       <c r="AB11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AC11" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>208</v>
+        <v>31</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AF11" s="1" t="s">
         <v>162</v>
@@ -3119,13 +3122,13 @@
         <v>165</v>
       </c>
       <c r="AX11" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY11" s="1">
         <v>100</v>
       </c>
       <c r="CE11" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:89" x14ac:dyDescent="0.25">
@@ -3133,13 +3136,13 @@
         <v>140</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>144</v>
@@ -3166,7 +3169,7 @@
         <v>151</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>153</v>
@@ -3178,7 +3181,7 @@
         <v>144</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>155</v>
@@ -3187,7 +3190,7 @@
         <v>156</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>153</v>
@@ -3196,7 +3199,7 @@
         <v>144</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="X12" s="1" t="s">
         <v>144</v>
@@ -3211,16 +3214,16 @@
         <v>157</v>
       </c>
       <c r="AB12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AC12" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AF12" s="1" t="s">
         <v>162</v>
@@ -3235,13 +3238,13 @@
         <v>165</v>
       </c>
       <c r="AX12" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY12" s="1">
         <v>100</v>
       </c>
       <c r="CE12" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:89" x14ac:dyDescent="0.25">
@@ -3249,13 +3252,13 @@
         <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>144</v>
@@ -3282,7 +3285,7 @@
         <v>151</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>153</v>
@@ -3294,7 +3297,7 @@
         <v>144</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>155</v>
@@ -3303,7 +3306,7 @@
         <v>156</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>153</v>
@@ -3312,7 +3315,7 @@
         <v>144</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>144</v>
@@ -3327,16 +3330,16 @@
         <v>157</v>
       </c>
       <c r="AB13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AC13" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>32</v>
+        <v>222</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AF13" s="1" t="s">
         <v>162</v>
@@ -3351,13 +3354,13 @@
         <v>165</v>
       </c>
       <c r="AX13" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY13" s="1">
         <v>100</v>
       </c>
       <c r="CE13" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:89" x14ac:dyDescent="0.25">
@@ -3365,13 +3368,13 @@
         <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>144</v>
@@ -3398,7 +3401,7 @@
         <v>151</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>153</v>
@@ -3410,7 +3413,7 @@
         <v>144</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>155</v>
@@ -3419,7 +3422,7 @@
         <v>156</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>153</v>
@@ -3428,7 +3431,7 @@
         <v>144</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="X14" s="1" t="s">
         <v>144</v>
@@ -3443,16 +3446,16 @@
         <v>157</v>
       </c>
       <c r="AB14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AC14" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AD14" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE14" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="AE14" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="AF14" s="1" t="s">
         <v>162</v>
@@ -3467,13 +3470,13 @@
         <v>165</v>
       </c>
       <c r="AX14" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY14" s="1">
         <v>100</v>
       </c>
       <c r="CE14" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:89" x14ac:dyDescent="0.25">
@@ -3481,13 +3484,13 @@
         <v>140</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>144</v>
@@ -3514,7 +3517,7 @@
         <v>151</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>153</v>
@@ -3526,7 +3529,7 @@
         <v>144</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>155</v>
@@ -3535,7 +3538,7 @@
         <v>156</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>153</v>
@@ -3544,7 +3547,7 @@
         <v>144</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X15" s="1" t="s">
         <v>144</v>
@@ -3559,13 +3562,13 @@
         <v>157</v>
       </c>
       <c r="AB15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AC15" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>31</v>
+        <v>238</v>
       </c>
       <c r="AE15" s="1" t="s">
         <v>239</v>
@@ -3583,7 +3586,7 @@
         <v>165</v>
       </c>
       <c r="AX15" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY15" s="1">
         <v>100</v>
@@ -3699,7 +3702,7 @@
         <v>165</v>
       </c>
       <c r="AX16" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY16" s="1">
         <v>100</v>
@@ -3815,7 +3818,7 @@
         <v>165</v>
       </c>
       <c r="AX17" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY17" s="1">
         <v>100</v>
@@ -3931,7 +3934,7 @@
         <v>165</v>
       </c>
       <c r="AX18" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY18" s="1">
         <v>100</v>
@@ -3951,7 +3954,7 @@
         <v>142</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>190</v>
+        <v>266</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>144</v>
@@ -3978,7 +3981,7 @@
         <v>151</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>153</v>
@@ -3990,7 +3993,7 @@
         <v>144</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="R19" s="1" t="s">
         <v>155</v>
@@ -3999,7 +4002,7 @@
         <v>156</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="U19" s="1" t="s">
         <v>153</v>
@@ -4008,7 +4011,7 @@
         <v>144</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="X19" s="1" t="s">
         <v>144</v>
@@ -4023,7 +4026,7 @@
         <v>157</v>
       </c>
       <c r="AB19" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="AC19" s="1" t="s">
         <v>159</v>
@@ -4032,7 +4035,7 @@
         <v>26</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="AF19" s="1" t="s">
         <v>162</v>
@@ -4047,13 +4050,13 @@
         <v>165</v>
       </c>
       <c r="AX19" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AY19" s="1">
         <v>100</v>
       </c>
       <c r="CE19" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>